<commit_message>
Updating the reproductive success data
</commit_message>
<xml_diff>
--- a/data/fitness_development/treatment_reproductive.xlsx
+++ b/data/fitness_development/treatment_reproductive.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster/data/fitness_development/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katiemillar/Documents/drosophila_project_2024/data/fitness_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DE4A98F-02C9-BB48-869B-3C6455806444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{93324C98-9B19-8245-92D5-4D443A33567E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{686100AC-FE20-0E41-BC7F-7F75F7633F5F}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{686100AC-FE20-0E41-BC7F-7F75F7633F5F}"/>
   </bookViews>
   <sheets>
     <sheet name="females" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="9">
   <si>
     <t>Conditioned focal female</t>
   </si>
@@ -759,7 +759,7 @@
         <v>9</v>
       </c>
       <c r="D19">
-        <f>SUM(C19)/3</f>
+        <f t="shared" ref="D19:D34" si="1">SUM(C19)/3</f>
         <v>3</v>
       </c>
       <c r="E19">
@@ -777,7 +777,7 @@
         <v>18</v>
       </c>
       <c r="D20">
-        <f>SUM(C20)/3</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E20">
@@ -795,7 +795,7 @@
         <v>14</v>
       </c>
       <c r="D21">
-        <f>SUM(C21)/3</f>
+        <f t="shared" si="1"/>
         <v>4.666666666666667</v>
       </c>
       <c r="E21">
@@ -813,7 +813,7 @@
         <v>10</v>
       </c>
       <c r="D22">
-        <f>SUM(C22)/3</f>
+        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="E22">
@@ -831,7 +831,7 @@
         <v>16</v>
       </c>
       <c r="D23">
-        <f>SUM(C23)/3</f>
+        <f t="shared" si="1"/>
         <v>5.333333333333333</v>
       </c>
       <c r="E23">
@@ -849,7 +849,7 @@
         <v>15</v>
       </c>
       <c r="D24">
-        <f>SUM(C24)/3</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="E24">
@@ -867,7 +867,7 @@
         <v>17</v>
       </c>
       <c r="D25">
-        <f>SUM(C25)/3</f>
+        <f t="shared" si="1"/>
         <v>5.666666666666667</v>
       </c>
       <c r="E25">
@@ -885,7 +885,7 @@
         <v>12</v>
       </c>
       <c r="D26">
-        <f>SUM(C26)/3</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E26">
@@ -903,7 +903,7 @@
         <v>8</v>
       </c>
       <c r="D27">
-        <f>SUM(C27)/3</f>
+        <f t="shared" si="1"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="E27">
@@ -921,7 +921,7 @@
         <v>5</v>
       </c>
       <c r="D28">
-        <f>SUM(C28)/3</f>
+        <f t="shared" si="1"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="E28">
@@ -939,7 +939,7 @@
         <v>18</v>
       </c>
       <c r="D29">
-        <f>SUM(C29)/3</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E29">
@@ -957,7 +957,7 @@
         <v>15</v>
       </c>
       <c r="D30">
-        <f>SUM(C30)/3</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="E30">
@@ -975,7 +975,7 @@
         <v>22</v>
       </c>
       <c r="D31">
-        <f>SUM(C31)/3</f>
+        <f t="shared" si="1"/>
         <v>7.333333333333333</v>
       </c>
       <c r="E31">
@@ -993,7 +993,7 @@
         <v>18</v>
       </c>
       <c r="D32">
-        <f>SUM(C32)/3</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E32">
@@ -1011,7 +1011,7 @@
         <v>17</v>
       </c>
       <c r="D33">
-        <f>SUM(C33)/3</f>
+        <f t="shared" si="1"/>
         <v>5.666666666666667</v>
       </c>
       <c r="E33">
@@ -1029,7 +1029,7 @@
         <v>1</v>
       </c>
       <c r="D34">
-        <f>SUM(C34)/3</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E34">
@@ -1058,7 +1058,7 @@
         <v>22</v>
       </c>
       <c r="D36">
-        <f t="shared" ref="D36:D69" si="1">SUM(C36)/3</f>
+        <f t="shared" ref="D36:D69" si="2">SUM(C36)/3</f>
         <v>7.333333333333333</v>
       </c>
       <c r="E36">
@@ -1087,7 +1087,7 @@
         <v>13</v>
       </c>
       <c r="D38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.333333333333333</v>
       </c>
       <c r="E38">
@@ -1105,7 +1105,7 @@
         <v>3</v>
       </c>
       <c r="D39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E39">
@@ -1145,7 +1145,7 @@
         <v>23</v>
       </c>
       <c r="D42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.666666666666667</v>
       </c>
       <c r="E42">
@@ -1163,7 +1163,7 @@
         <v>20</v>
       </c>
       <c r="D43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.666666666666667</v>
       </c>
       <c r="E43">
@@ -1192,7 +1192,7 @@
         <v>16</v>
       </c>
       <c r="D45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.333333333333333</v>
       </c>
       <c r="E45">
@@ -1221,7 +1221,7 @@
         <v>0</v>
       </c>
       <c r="D47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E47">
@@ -1239,7 +1239,7 @@
         <v>20</v>
       </c>
       <c r="D48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.666666666666667</v>
       </c>
       <c r="E48">
@@ -1257,7 +1257,7 @@
         <v>8</v>
       </c>
       <c r="D49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="E49">
@@ -1275,7 +1275,7 @@
         <v>5</v>
       </c>
       <c r="D50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="E50">
@@ -1293,7 +1293,7 @@
         <v>18</v>
       </c>
       <c r="D51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E51">
@@ -1311,7 +1311,7 @@
         <v>9</v>
       </c>
       <c r="D52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="E52">
@@ -1329,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="D53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E53">
@@ -1347,7 +1347,7 @@
         <v>24</v>
       </c>
       <c r="D54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="E54">
@@ -1387,7 +1387,7 @@
         <v>13</v>
       </c>
       <c r="D57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.333333333333333</v>
       </c>
       <c r="E57">
@@ -1405,7 +1405,7 @@
         <v>5</v>
       </c>
       <c r="D58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="E58">
@@ -1423,7 +1423,7 @@
         <v>4</v>
       </c>
       <c r="D59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="E59">
@@ -1441,7 +1441,7 @@
         <v>19</v>
       </c>
       <c r="D60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.333333333333333</v>
       </c>
       <c r="E60">
@@ -1470,7 +1470,7 @@
         <v>5</v>
       </c>
       <c r="D62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="E62">
@@ -1517,7 +1517,7 @@
         <v>10</v>
       </c>
       <c r="D65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="E65">
@@ -1535,7 +1535,7 @@
         <v>14</v>
       </c>
       <c r="D66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.666666666666667</v>
       </c>
       <c r="E66">
@@ -1553,7 +1553,7 @@
         <v>13</v>
       </c>
       <c r="D67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.333333333333333</v>
       </c>
       <c r="E67">
@@ -1571,7 +1571,7 @@
         <v>5</v>
       </c>
       <c r="D68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="E68">
@@ -1589,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="D69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E69">
@@ -1680,7 +1680,7 @@
         <v>18</v>
       </c>
       <c r="D76">
-        <f t="shared" ref="D71:D86" si="2">SUM(C76)/4</f>
+        <f t="shared" ref="D76:D85" si="3">SUM(C76)/4</f>
         <v>4.5</v>
       </c>
       <c r="E76">
@@ -1698,7 +1698,7 @@
         <v>12</v>
       </c>
       <c r="D77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E77">
@@ -1793,7 +1793,7 @@
         <v>8</v>
       </c>
       <c r="D85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E85">
@@ -2011,10 +2011,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A020D176-250D-0E4A-BAEF-162FCAF5B741}">
-  <dimension ref="A1:E160"/>
+  <dimension ref="A1:E319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="165" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="165" workbookViewId="0">
+      <selection activeCell="G313" sqref="G313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2054,7 +2054,7 @@
         <v>18</v>
       </c>
       <c r="E2">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2072,7 +2072,7 @@
         <v>11.333333333333334</v>
       </c>
       <c r="E3">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2086,11 +2086,11 @@
         <v>26</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D27" si="0">SUM(C4)/3</f>
+        <f t="shared" ref="D4:D26" si="0">SUM(C4)/3</f>
         <v>8.6666666666666661</v>
       </c>
       <c r="E4">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2108,7 +2108,7 @@
         <v>13</v>
       </c>
       <c r="E5">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2126,7 +2126,7 @@
         <v>7.666666666666667</v>
       </c>
       <c r="E6">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2144,7 +2144,7 @@
         <v>11</v>
       </c>
       <c r="E7">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2162,7 +2162,7 @@
         <v>6.333333333333333</v>
       </c>
       <c r="E8">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2180,7 +2180,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2198,7 +2198,7 @@
         <v>7.333333333333333</v>
       </c>
       <c r="E10">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2209,7 +2209,7 @@
         <v>27</v>
       </c>
       <c r="E11">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2227,7 +2227,7 @@
         <v>14.333333333333334</v>
       </c>
       <c r="E12">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2245,7 +2245,7 @@
         <v>12</v>
       </c>
       <c r="E13">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2263,7 +2263,7 @@
         <v>14</v>
       </c>
       <c r="E14">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2281,7 +2281,7 @@
         <v>9.3333333333333339</v>
       </c>
       <c r="E15">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2299,7 +2299,7 @@
         <v>13</v>
       </c>
       <c r="E16">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -2317,7 +2317,7 @@
         <v>12</v>
       </c>
       <c r="E17">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -2335,7 +2335,7 @@
         <v>11.333333333333334</v>
       </c>
       <c r="E18">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -2353,7 +2353,7 @@
         <v>11</v>
       </c>
       <c r="E19">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2371,7 +2371,7 @@
         <v>11</v>
       </c>
       <c r="E20">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2389,7 +2389,7 @@
         <v>14.333333333333334</v>
       </c>
       <c r="E21">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -2400,7 +2400,7 @@
         <v>38</v>
       </c>
       <c r="E22">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -2418,7 +2418,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -2436,7 +2436,7 @@
         <v>24</v>
       </c>
       <c r="E24">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -2454,7 +2454,7 @@
         <v>9.6666666666666661</v>
       </c>
       <c r="E25">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -2472,7 +2472,7 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -2483,7 +2483,7 @@
         <v>43</v>
       </c>
       <c r="E27">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -2494,7 +2494,7 @@
         <v>44</v>
       </c>
       <c r="E28">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -2508,11 +2508,11 @@
         <v>43</v>
       </c>
       <c r="D29">
-        <f>SUM(C29)/3</f>
+        <f t="shared" ref="D29:D56" si="1">SUM(C29)/3</f>
         <v>14.333333333333334</v>
       </c>
       <c r="E29">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -2526,11 +2526,11 @@
         <v>29</v>
       </c>
       <c r="D30">
-        <f>SUM(C30)/3</f>
+        <f t="shared" si="1"/>
         <v>9.6666666666666661</v>
       </c>
       <c r="E30">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -2544,11 +2544,11 @@
         <v>19</v>
       </c>
       <c r="D31">
-        <f>SUM(C31)/3</f>
+        <f t="shared" si="1"/>
         <v>6.333333333333333</v>
       </c>
       <c r="E31">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -2562,11 +2562,11 @@
         <v>29</v>
       </c>
       <c r="D32">
-        <f>SUM(C32)/3</f>
+        <f t="shared" si="1"/>
         <v>9.6666666666666661</v>
       </c>
       <c r="E32">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -2580,11 +2580,11 @@
         <v>43</v>
       </c>
       <c r="D33">
-        <f>SUM(C33)/3</f>
+        <f t="shared" si="1"/>
         <v>14.333333333333334</v>
       </c>
       <c r="E33">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -2598,11 +2598,11 @@
         <v>23</v>
       </c>
       <c r="D34">
-        <f>SUM(C34)/3</f>
+        <f t="shared" si="1"/>
         <v>7.666666666666667</v>
       </c>
       <c r="E34">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -2616,11 +2616,11 @@
         <v>46</v>
       </c>
       <c r="D35">
-        <f>SUM(C35)/3</f>
+        <f t="shared" si="1"/>
         <v>15.333333333333334</v>
       </c>
       <c r="E35">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -2634,11 +2634,11 @@
         <v>60</v>
       </c>
       <c r="D36">
-        <f>SUM(C36)/3</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="E36">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -2652,11 +2652,11 @@
         <v>28</v>
       </c>
       <c r="D37">
-        <f>SUM(C37)/3</f>
+        <f t="shared" si="1"/>
         <v>9.3333333333333339</v>
       </c>
       <c r="E37">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -2670,11 +2670,11 @@
         <v>52</v>
       </c>
       <c r="D38">
-        <f>SUM(C38)/3</f>
+        <f t="shared" si="1"/>
         <v>17.333333333333332</v>
       </c>
       <c r="E38">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -2688,11 +2688,11 @@
         <v>22</v>
       </c>
       <c r="D39">
-        <f>SUM(C39)/3</f>
+        <f t="shared" si="1"/>
         <v>7.333333333333333</v>
       </c>
       <c r="E39">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -2706,11 +2706,11 @@
         <v>47</v>
       </c>
       <c r="D40">
-        <f>SUM(C40)/3</f>
+        <f t="shared" si="1"/>
         <v>15.666666666666666</v>
       </c>
       <c r="E40">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -2724,11 +2724,11 @@
         <v>38</v>
       </c>
       <c r="D41">
-        <f>SUM(C41)/3</f>
+        <f t="shared" si="1"/>
         <v>12.666666666666666</v>
       </c>
       <c r="E41">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2742,11 +2742,11 @@
         <v>27</v>
       </c>
       <c r="D42">
-        <f>SUM(C42)/3</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="E42">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -2760,11 +2760,11 @@
         <v>52</v>
       </c>
       <c r="D43">
-        <f>SUM(C43)/3</f>
+        <f t="shared" si="1"/>
         <v>17.333333333333332</v>
       </c>
       <c r="E43">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -2778,11 +2778,11 @@
         <v>35</v>
       </c>
       <c r="D44">
-        <f>SUM(C44)/3</f>
+        <f t="shared" si="1"/>
         <v>11.666666666666666</v>
       </c>
       <c r="E44">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -2796,11 +2796,11 @@
         <v>50</v>
       </c>
       <c r="D45">
-        <f>SUM(C45)/3</f>
+        <f t="shared" si="1"/>
         <v>16.666666666666668</v>
       </c>
       <c r="E45">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -2814,11 +2814,11 @@
         <v>48</v>
       </c>
       <c r="D46">
-        <f>SUM(C46)/3</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="E46">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -2832,11 +2832,11 @@
         <v>28</v>
       </c>
       <c r="D47">
-        <f>SUM(C47)/3</f>
+        <f t="shared" si="1"/>
         <v>9.3333333333333339</v>
       </c>
       <c r="E47">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -2850,11 +2850,11 @@
         <v>60</v>
       </c>
       <c r="D48">
-        <f>SUM(C48)/3</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="E48">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -2868,11 +2868,11 @@
         <v>53</v>
       </c>
       <c r="D49">
-        <f>SUM(C49)/3</f>
+        <f t="shared" si="1"/>
         <v>17.666666666666668</v>
       </c>
       <c r="E49">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -2886,11 +2886,11 @@
         <v>57</v>
       </c>
       <c r="D50">
-        <f>SUM(C50)/3</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="E50">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -2904,11 +2904,11 @@
         <v>65</v>
       </c>
       <c r="D51">
-        <f>SUM(C51)/3</f>
+        <f t="shared" si="1"/>
         <v>21.666666666666668</v>
       </c>
       <c r="E51">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -2922,11 +2922,11 @@
         <v>61</v>
       </c>
       <c r="D52">
-        <f>SUM(C52)/3</f>
+        <f t="shared" si="1"/>
         <v>20.333333333333332</v>
       </c>
       <c r="E52">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -2940,11 +2940,11 @@
         <v>51</v>
       </c>
       <c r="D53">
-        <f>SUM(C53)/3</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="E53">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -2958,11 +2958,11 @@
         <v>22</v>
       </c>
       <c r="D54">
-        <f>SUM(C54)/3</f>
+        <f t="shared" si="1"/>
         <v>7.333333333333333</v>
       </c>
       <c r="E54">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -2976,11 +2976,11 @@
         <v>10</v>
       </c>
       <c r="D55">
-        <f>SUM(C55)/3</f>
+        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="E55">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -2994,11 +2994,11 @@
         <v>21</v>
       </c>
       <c r="D56">
-        <f>SUM(C56)/3</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="E56">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -3009,7 +3009,7 @@
         <v>20</v>
       </c>
       <c r="E57">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -3023,11 +3023,11 @@
         <v>25</v>
       </c>
       <c r="D58">
-        <f t="shared" ref="D57:D109" si="1">SUM(C58)/3</f>
+        <f t="shared" ref="D58:D107" si="2">SUM(C58)/3</f>
         <v>8.3333333333333339</v>
       </c>
       <c r="E58">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -3041,11 +3041,11 @@
         <v>27</v>
       </c>
       <c r="D59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="E59">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -3059,11 +3059,11 @@
         <v>16</v>
       </c>
       <c r="D60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.333333333333333</v>
       </c>
       <c r="E60">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -3077,11 +3077,11 @@
         <v>1</v>
       </c>
       <c r="D61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E61">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -3092,7 +3092,7 @@
         <v>25</v>
       </c>
       <c r="E62">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -3106,11 +3106,11 @@
         <v>22</v>
       </c>
       <c r="D63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.333333333333333</v>
       </c>
       <c r="E63">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -3124,11 +3124,11 @@
         <v>9</v>
       </c>
       <c r="D64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="E64">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -3142,11 +3142,11 @@
         <v>39</v>
       </c>
       <c r="D65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="E65">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -3160,11 +3160,11 @@
         <v>25</v>
       </c>
       <c r="D66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.3333333333333339</v>
       </c>
       <c r="E66">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -3178,11 +3178,11 @@
         <v>25</v>
       </c>
       <c r="D67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.3333333333333339</v>
       </c>
       <c r="E67">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -3196,11 +3196,11 @@
         <v>42</v>
       </c>
       <c r="D68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="E68">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -3214,11 +3214,11 @@
         <v>31</v>
       </c>
       <c r="D69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10.333333333333334</v>
       </c>
       <c r="E69">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -3232,11 +3232,11 @@
         <v>37</v>
       </c>
       <c r="D70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.333333333333334</v>
       </c>
       <c r="E70">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -3250,11 +3250,11 @@
         <v>37</v>
       </c>
       <c r="D71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.333333333333334</v>
       </c>
       <c r="E71">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -3268,11 +3268,11 @@
         <v>27</v>
       </c>
       <c r="D72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="E72">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -3286,11 +3286,11 @@
         <v>42</v>
       </c>
       <c r="D73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="E73">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -3304,11 +3304,11 @@
         <v>36</v>
       </c>
       <c r="D74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="E74">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -3322,11 +3322,11 @@
         <v>19</v>
       </c>
       <c r="D75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.333333333333333</v>
       </c>
       <c r="E75">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -3340,11 +3340,11 @@
         <v>0</v>
       </c>
       <c r="D76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E76">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -3358,11 +3358,11 @@
         <v>47</v>
       </c>
       <c r="D77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15.666666666666666</v>
       </c>
       <c r="E77">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -3376,11 +3376,11 @@
         <v>10</v>
       </c>
       <c r="D78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="E78">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -3394,11 +3394,11 @@
         <v>0</v>
       </c>
       <c r="D79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E79">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -3409,7 +3409,7 @@
         <v>43</v>
       </c>
       <c r="E80">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -3423,11 +3423,11 @@
         <v>39</v>
       </c>
       <c r="D81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="E81">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -3438,7 +3438,7 @@
         <v>62</v>
       </c>
       <c r="E82">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -3452,11 +3452,11 @@
         <v>22</v>
       </c>
       <c r="D83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.333333333333333</v>
       </c>
       <c r="E83">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -3470,11 +3470,11 @@
         <v>42</v>
       </c>
       <c r="D84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="E84">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -3485,7 +3485,7 @@
         <v>65</v>
       </c>
       <c r="E85">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -3499,11 +3499,11 @@
         <v>33</v>
       </c>
       <c r="D86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="E86">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -3514,7 +3514,7 @@
         <v>67</v>
       </c>
       <c r="E87">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -3528,11 +3528,11 @@
         <v>25</v>
       </c>
       <c r="D88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.3333333333333339</v>
       </c>
       <c r="E88">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -3546,11 +3546,11 @@
         <v>26</v>
       </c>
       <c r="D89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.6666666666666661</v>
       </c>
       <c r="E89">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -3564,11 +3564,11 @@
         <v>51</v>
       </c>
       <c r="D90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="E90">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -3582,11 +3582,11 @@
         <v>40</v>
       </c>
       <c r="D91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.333333333333334</v>
       </c>
       <c r="E91">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -3600,11 +3600,11 @@
         <v>45</v>
       </c>
       <c r="D92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="E92">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -3615,7 +3615,7 @@
         <v>73</v>
       </c>
       <c r="E93">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -3629,11 +3629,11 @@
         <v>34</v>
       </c>
       <c r="D94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11.333333333333334</v>
       </c>
       <c r="E94">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -3647,11 +3647,11 @@
         <v>48</v>
       </c>
       <c r="D95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="E95">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -3665,11 +3665,11 @@
         <v>40</v>
       </c>
       <c r="D96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.333333333333334</v>
       </c>
       <c r="E96">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -3683,11 +3683,11 @@
         <v>30</v>
       </c>
       <c r="D97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="E97">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -3701,11 +3701,11 @@
         <v>44</v>
       </c>
       <c r="D98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14.666666666666666</v>
       </c>
       <c r="E98">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -3719,11 +3719,11 @@
         <v>53</v>
       </c>
       <c r="D99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17.666666666666668</v>
       </c>
       <c r="E99">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -3737,11 +3737,11 @@
         <v>40</v>
       </c>
       <c r="D100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.333333333333334</v>
       </c>
       <c r="E100">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -3755,11 +3755,11 @@
         <v>47</v>
       </c>
       <c r="D101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15.666666666666666</v>
       </c>
       <c r="E101">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -3773,11 +3773,11 @@
         <v>10</v>
       </c>
       <c r="D102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="E102">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -3791,11 +3791,11 @@
         <v>53</v>
       </c>
       <c r="D103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17.666666666666668</v>
       </c>
       <c r="E103">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -3809,11 +3809,11 @@
         <v>32</v>
       </c>
       <c r="D104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10.666666666666666</v>
       </c>
       <c r="E104">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -3827,11 +3827,11 @@
         <v>47</v>
       </c>
       <c r="D105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15.666666666666666</v>
       </c>
       <c r="E105">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -3845,11 +3845,11 @@
         <v>47</v>
       </c>
       <c r="D106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15.666666666666666</v>
       </c>
       <c r="E106">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -3863,11 +3863,11 @@
         <v>41</v>
       </c>
       <c r="D107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.666666666666666</v>
       </c>
       <c r="E107">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -3932,7 +3932,7 @@
         <v>52</v>
       </c>
       <c r="D112">
-        <f t="shared" ref="D110:D160" si="2">SUM(C112)/4</f>
+        <f t="shared" ref="D112:D160" si="3">SUM(C112)/4</f>
         <v>13</v>
       </c>
       <c r="E112">
@@ -3950,7 +3950,7 @@
         <v>0</v>
       </c>
       <c r="D113">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E113">
@@ -3968,7 +3968,7 @@
         <v>59</v>
       </c>
       <c r="D114">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14.75</v>
       </c>
       <c r="E114">
@@ -3997,7 +3997,7 @@
         <v>35</v>
       </c>
       <c r="D116">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.75</v>
       </c>
       <c r="E116">
@@ -4015,7 +4015,7 @@
         <v>26</v>
       </c>
       <c r="D117">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.5</v>
       </c>
       <c r="E117">
@@ -4055,7 +4055,7 @@
         <v>33</v>
       </c>
       <c r="D120">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.25</v>
       </c>
       <c r="E120">
@@ -4073,7 +4073,7 @@
         <v>6</v>
       </c>
       <c r="D121">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="E121">
@@ -4091,7 +4091,7 @@
         <v>35</v>
       </c>
       <c r="D122">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.75</v>
       </c>
       <c r="E122">
@@ -4120,7 +4120,7 @@
         <v>36</v>
       </c>
       <c r="D124">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="E124">
@@ -4138,7 +4138,7 @@
         <v>35</v>
       </c>
       <c r="D125">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.75</v>
       </c>
       <c r="E125">
@@ -4167,7 +4167,7 @@
         <v>45</v>
       </c>
       <c r="D127">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11.25</v>
       </c>
       <c r="E127">
@@ -4185,7 +4185,7 @@
         <v>0</v>
       </c>
       <c r="D128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E128">
@@ -4214,7 +4214,7 @@
         <v>43</v>
       </c>
       <c r="D130">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10.75</v>
       </c>
       <c r="E130">
@@ -4243,7 +4243,7 @@
         <v>6</v>
       </c>
       <c r="D132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="E132">
@@ -4272,7 +4272,7 @@
         <v>38</v>
       </c>
       <c r="D134">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.5</v>
       </c>
       <c r="E134">
@@ -4301,7 +4301,7 @@
         <v>0</v>
       </c>
       <c r="D136">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E136">
@@ -4341,7 +4341,7 @@
         <v>52</v>
       </c>
       <c r="D139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="E139">
@@ -4370,7 +4370,7 @@
         <v>55</v>
       </c>
       <c r="D141">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.75</v>
       </c>
       <c r="E141">
@@ -4388,7 +4388,7 @@
         <v>40</v>
       </c>
       <c r="D142">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="E142">
@@ -4417,7 +4417,7 @@
         <v>41</v>
       </c>
       <c r="D144">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10.25</v>
       </c>
       <c r="E144">
@@ -4435,7 +4435,7 @@
         <v>42</v>
       </c>
       <c r="D145">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10.5</v>
       </c>
       <c r="E145">
@@ -4486,7 +4486,7 @@
         <v>62</v>
       </c>
       <c r="D149">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
       <c r="E149">
@@ -4504,7 +4504,7 @@
         <v>12</v>
       </c>
       <c r="D150">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E150">
@@ -4522,7 +4522,7 @@
         <v>21</v>
       </c>
       <c r="D151">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.25</v>
       </c>
       <c r="E151">
@@ -4551,7 +4551,7 @@
         <v>18</v>
       </c>
       <c r="D153">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.5</v>
       </c>
       <c r="E153">
@@ -4569,7 +4569,7 @@
         <v>13</v>
       </c>
       <c r="D154">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.25</v>
       </c>
       <c r="E154">
@@ -4587,7 +4587,7 @@
         <v>50</v>
       </c>
       <c r="D155">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="E155">
@@ -4605,7 +4605,7 @@
         <v>47</v>
       </c>
       <c r="D156">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11.75</v>
       </c>
       <c r="E156">
@@ -4634,7 +4634,7 @@
         <v>41</v>
       </c>
       <c r="D158">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10.25</v>
       </c>
       <c r="E158">
@@ -4663,11 +4663,2316 @@
         <v>33</v>
       </c>
       <c r="D160">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.25</v>
       </c>
       <c r="E160">
         <v>22</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>1</v>
+      </c>
+      <c r="B161">
+        <v>18</v>
+      </c>
+      <c r="C161">
+        <v>36</v>
+      </c>
+      <c r="D161">
+        <f>SUM(C161)/3</f>
+        <v>12</v>
+      </c>
+      <c r="E161">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>1</v>
+      </c>
+      <c r="B162">
+        <v>19</v>
+      </c>
+      <c r="E162">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>1</v>
+      </c>
+      <c r="B163">
+        <v>20</v>
+      </c>
+      <c r="E163">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>1</v>
+      </c>
+      <c r="B164">
+        <v>21</v>
+      </c>
+      <c r="E164">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>1</v>
+      </c>
+      <c r="B165">
+        <v>22</v>
+      </c>
+      <c r="C165">
+        <v>26</v>
+      </c>
+      <c r="D165">
+        <f t="shared" ref="D165:D213" si="4">SUM(C165)/3</f>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="E165">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>1</v>
+      </c>
+      <c r="B166">
+        <v>23</v>
+      </c>
+      <c r="C166">
+        <v>3</v>
+      </c>
+      <c r="D166">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E166">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>1</v>
+      </c>
+      <c r="B167">
+        <v>24</v>
+      </c>
+      <c r="E167">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>1</v>
+      </c>
+      <c r="B168">
+        <v>25</v>
+      </c>
+      <c r="E168">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>1</v>
+      </c>
+      <c r="B169">
+        <v>26</v>
+      </c>
+      <c r="C169">
+        <v>11</v>
+      </c>
+      <c r="D169">
+        <f t="shared" si="4"/>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="E169">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>1</v>
+      </c>
+      <c r="B170">
+        <v>27</v>
+      </c>
+      <c r="C170">
+        <v>20</v>
+      </c>
+      <c r="D170">
+        <f t="shared" si="4"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="E170">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>1</v>
+      </c>
+      <c r="B171">
+        <v>28</v>
+      </c>
+      <c r="E171">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>1</v>
+      </c>
+      <c r="B172">
+        <v>29</v>
+      </c>
+      <c r="E172">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>1</v>
+      </c>
+      <c r="B173">
+        <v>30</v>
+      </c>
+      <c r="C173">
+        <v>19</v>
+      </c>
+      <c r="D173">
+        <f t="shared" si="4"/>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="E173">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>1</v>
+      </c>
+      <c r="B174">
+        <v>31</v>
+      </c>
+      <c r="C174">
+        <v>8</v>
+      </c>
+      <c r="D174">
+        <f t="shared" si="4"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="E174">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>1</v>
+      </c>
+      <c r="B175">
+        <v>32</v>
+      </c>
+      <c r="C175">
+        <v>34</v>
+      </c>
+      <c r="D175">
+        <f t="shared" si="4"/>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="E175">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>1</v>
+      </c>
+      <c r="B176">
+        <v>33</v>
+      </c>
+      <c r="E176">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>1</v>
+      </c>
+      <c r="B177">
+        <v>34</v>
+      </c>
+      <c r="C177">
+        <v>26</v>
+      </c>
+      <c r="D177">
+        <f t="shared" si="4"/>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="E177">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>1</v>
+      </c>
+      <c r="B178">
+        <v>35</v>
+      </c>
+      <c r="C178">
+        <v>33</v>
+      </c>
+      <c r="D178">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="E178">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>1</v>
+      </c>
+      <c r="B179">
+        <v>36</v>
+      </c>
+      <c r="E179">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>1</v>
+      </c>
+      <c r="B180">
+        <v>37</v>
+      </c>
+      <c r="C180">
+        <v>49</v>
+      </c>
+      <c r="D180">
+        <f t="shared" si="4"/>
+        <v>16.333333333333332</v>
+      </c>
+      <c r="E180">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>1</v>
+      </c>
+      <c r="B181">
+        <v>38</v>
+      </c>
+      <c r="E181">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>1</v>
+      </c>
+      <c r="B182">
+        <v>39</v>
+      </c>
+      <c r="E182">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>1</v>
+      </c>
+      <c r="B183">
+        <v>40</v>
+      </c>
+      <c r="E183">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>1</v>
+      </c>
+      <c r="B184">
+        <v>41</v>
+      </c>
+      <c r="E184">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>1</v>
+      </c>
+      <c r="B185">
+        <v>42</v>
+      </c>
+      <c r="C185">
+        <v>0</v>
+      </c>
+      <c r="D185">
+        <v>0</v>
+      </c>
+      <c r="E185">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>1</v>
+      </c>
+      <c r="B186">
+        <v>43</v>
+      </c>
+      <c r="E186">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>1</v>
+      </c>
+      <c r="B187">
+        <v>44</v>
+      </c>
+      <c r="C187">
+        <v>35</v>
+      </c>
+      <c r="D187">
+        <f t="shared" si="4"/>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="E187">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>3</v>
+      </c>
+      <c r="B188">
+        <v>62</v>
+      </c>
+      <c r="E188">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>3</v>
+      </c>
+      <c r="B189">
+        <v>63</v>
+      </c>
+      <c r="C189">
+        <v>0</v>
+      </c>
+      <c r="D189">
+        <v>0</v>
+      </c>
+      <c r="E189">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>3</v>
+      </c>
+      <c r="B190">
+        <v>64</v>
+      </c>
+      <c r="E190">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>3</v>
+      </c>
+      <c r="B191">
+        <v>65</v>
+      </c>
+      <c r="E191">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>3</v>
+      </c>
+      <c r="B192">
+        <v>66</v>
+      </c>
+      <c r="C192">
+        <v>38</v>
+      </c>
+      <c r="D192">
+        <f t="shared" si="4"/>
+        <v>12.666666666666666</v>
+      </c>
+      <c r="E192">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>3</v>
+      </c>
+      <c r="B193">
+        <v>67</v>
+      </c>
+      <c r="E193">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>3</v>
+      </c>
+      <c r="B194">
+        <v>68</v>
+      </c>
+      <c r="C194">
+        <v>20</v>
+      </c>
+      <c r="D194">
+        <f t="shared" si="4"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="E194">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>3</v>
+      </c>
+      <c r="B195">
+        <v>69</v>
+      </c>
+      <c r="C195">
+        <v>47</v>
+      </c>
+      <c r="D195">
+        <f t="shared" si="4"/>
+        <v>15.666666666666666</v>
+      </c>
+      <c r="E195">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>3</v>
+      </c>
+      <c r="B196">
+        <v>70</v>
+      </c>
+      <c r="C196">
+        <v>26</v>
+      </c>
+      <c r="D196">
+        <f t="shared" si="4"/>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="E196">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>3</v>
+      </c>
+      <c r="B197">
+        <v>71</v>
+      </c>
+      <c r="C197">
+        <v>37</v>
+      </c>
+      <c r="D197">
+        <f t="shared" si="4"/>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="E197">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>3</v>
+      </c>
+      <c r="B198">
+        <v>72</v>
+      </c>
+      <c r="E198">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>3</v>
+      </c>
+      <c r="B199">
+        <v>73</v>
+      </c>
+      <c r="E199">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>3</v>
+      </c>
+      <c r="B200">
+        <v>74</v>
+      </c>
+      <c r="E200">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>3</v>
+      </c>
+      <c r="B201">
+        <v>75</v>
+      </c>
+      <c r="E201">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>3</v>
+      </c>
+      <c r="B202">
+        <v>76</v>
+      </c>
+      <c r="C202">
+        <v>35</v>
+      </c>
+      <c r="D202">
+        <f t="shared" si="4"/>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="E202">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>3</v>
+      </c>
+      <c r="B203">
+        <v>77</v>
+      </c>
+      <c r="C203">
+        <v>1</v>
+      </c>
+      <c r="D203">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E203">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>3</v>
+      </c>
+      <c r="B204">
+        <v>78</v>
+      </c>
+      <c r="C204">
+        <v>0</v>
+      </c>
+      <c r="D204">
+        <v>0</v>
+      </c>
+      <c r="E204">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>3</v>
+      </c>
+      <c r="B205">
+        <v>79</v>
+      </c>
+      <c r="E205">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>3</v>
+      </c>
+      <c r="B206">
+        <v>80</v>
+      </c>
+      <c r="C206">
+        <v>19</v>
+      </c>
+      <c r="D206">
+        <f t="shared" si="4"/>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="E206">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>3</v>
+      </c>
+      <c r="B207">
+        <v>81</v>
+      </c>
+      <c r="C207">
+        <v>8</v>
+      </c>
+      <c r="D207">
+        <f t="shared" si="4"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="E207">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>3</v>
+      </c>
+      <c r="B208">
+        <v>82</v>
+      </c>
+      <c r="C208">
+        <v>48</v>
+      </c>
+      <c r="D208">
+        <f>SUM(C208)/3</f>
+        <v>16</v>
+      </c>
+      <c r="E208">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>3</v>
+      </c>
+      <c r="B209">
+        <v>83</v>
+      </c>
+      <c r="C209">
+        <v>45</v>
+      </c>
+      <c r="D209">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="E209">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>3</v>
+      </c>
+      <c r="B210">
+        <v>84</v>
+      </c>
+      <c r="E210">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>3</v>
+      </c>
+      <c r="B211">
+        <v>85</v>
+      </c>
+      <c r="C211">
+        <v>49</v>
+      </c>
+      <c r="D211">
+        <f t="shared" si="4"/>
+        <v>16.333333333333332</v>
+      </c>
+      <c r="E211">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>3</v>
+      </c>
+      <c r="B212">
+        <v>86</v>
+      </c>
+      <c r="E212">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>3</v>
+      </c>
+      <c r="B213">
+        <v>87</v>
+      </c>
+      <c r="C213">
+        <v>30</v>
+      </c>
+      <c r="D213">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="E213">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>1</v>
+      </c>
+      <c r="B214">
+        <v>18</v>
+      </c>
+      <c r="E214">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>1</v>
+      </c>
+      <c r="B215">
+        <v>19</v>
+      </c>
+      <c r="C215">
+        <v>40</v>
+      </c>
+      <c r="D215">
+        <f>SUM(C215)/3</f>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="E215">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>1</v>
+      </c>
+      <c r="B216">
+        <v>20</v>
+      </c>
+      <c r="D216">
+        <f t="shared" ref="D216:D266" si="5">SUM(C216)/3</f>
+        <v>0</v>
+      </c>
+      <c r="E216">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>1</v>
+      </c>
+      <c r="B217">
+        <v>21</v>
+      </c>
+      <c r="D217">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E217">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>1</v>
+      </c>
+      <c r="B218">
+        <v>22</v>
+      </c>
+      <c r="C218">
+        <v>43</v>
+      </c>
+      <c r="D218">
+        <f t="shared" si="5"/>
+        <v>14.333333333333334</v>
+      </c>
+      <c r="E218">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>1</v>
+      </c>
+      <c r="B219">
+        <v>23</v>
+      </c>
+      <c r="D219">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E219">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>1</v>
+      </c>
+      <c r="B220">
+        <v>24</v>
+      </c>
+      <c r="D220">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E220">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>1</v>
+      </c>
+      <c r="B221">
+        <v>25</v>
+      </c>
+      <c r="D221">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E221">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>1</v>
+      </c>
+      <c r="B222">
+        <v>26</v>
+      </c>
+      <c r="C222">
+        <v>12</v>
+      </c>
+      <c r="D222">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="E222">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>1</v>
+      </c>
+      <c r="B223">
+        <v>27</v>
+      </c>
+      <c r="C223">
+        <v>24</v>
+      </c>
+      <c r="D223">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="E223">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>1</v>
+      </c>
+      <c r="B224">
+        <v>28</v>
+      </c>
+      <c r="D224">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E224">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>1</v>
+      </c>
+      <c r="B225">
+        <v>29</v>
+      </c>
+      <c r="D225">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E225">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>1</v>
+      </c>
+      <c r="B226">
+        <v>30</v>
+      </c>
+      <c r="C226">
+        <v>28</v>
+      </c>
+      <c r="D226">
+        <f t="shared" si="5"/>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="E226">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>1</v>
+      </c>
+      <c r="B227">
+        <v>31</v>
+      </c>
+      <c r="C227">
+        <v>22</v>
+      </c>
+      <c r="D227">
+        <f t="shared" si="5"/>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="E227">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>1</v>
+      </c>
+      <c r="B228">
+        <v>32</v>
+      </c>
+      <c r="C228">
+        <v>44</v>
+      </c>
+      <c r="D228">
+        <f t="shared" si="5"/>
+        <v>14.666666666666666</v>
+      </c>
+      <c r="E228">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>1</v>
+      </c>
+      <c r="B229">
+        <v>33</v>
+      </c>
+      <c r="D229">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E229">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>1</v>
+      </c>
+      <c r="B230">
+        <v>34</v>
+      </c>
+      <c r="D230">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E230">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>1</v>
+      </c>
+      <c r="B231">
+        <v>35</v>
+      </c>
+      <c r="C231">
+        <v>47</v>
+      </c>
+      <c r="D231">
+        <f t="shared" si="5"/>
+        <v>15.666666666666666</v>
+      </c>
+      <c r="E231">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>1</v>
+      </c>
+      <c r="B232">
+        <v>36</v>
+      </c>
+      <c r="D232">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E232">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>1</v>
+      </c>
+      <c r="B233">
+        <v>37</v>
+      </c>
+      <c r="C233">
+        <v>45</v>
+      </c>
+      <c r="D233">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="E233">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>1</v>
+      </c>
+      <c r="B234">
+        <v>38</v>
+      </c>
+      <c r="D234">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E234">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>1</v>
+      </c>
+      <c r="B235">
+        <v>39</v>
+      </c>
+      <c r="D235">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E235">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>1</v>
+      </c>
+      <c r="B236">
+        <v>40</v>
+      </c>
+      <c r="C236">
+        <v>57</v>
+      </c>
+      <c r="D236">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="E236">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>1</v>
+      </c>
+      <c r="B237">
+        <v>41</v>
+      </c>
+      <c r="E237">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>1</v>
+      </c>
+      <c r="B238">
+        <v>42</v>
+      </c>
+      <c r="E238">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>1</v>
+      </c>
+      <c r="B239">
+        <v>43</v>
+      </c>
+      <c r="E239">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>1</v>
+      </c>
+      <c r="B240">
+        <v>44</v>
+      </c>
+      <c r="C240">
+        <v>44</v>
+      </c>
+      <c r="D240">
+        <f t="shared" si="5"/>
+        <v>14.666666666666666</v>
+      </c>
+      <c r="E240">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>3</v>
+      </c>
+      <c r="B241">
+        <v>62</v>
+      </c>
+      <c r="E241">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>3</v>
+      </c>
+      <c r="B242">
+        <v>63</v>
+      </c>
+      <c r="C242">
+        <v>0</v>
+      </c>
+      <c r="D242">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E242">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>3</v>
+      </c>
+      <c r="B243">
+        <v>64</v>
+      </c>
+      <c r="E243">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>3</v>
+      </c>
+      <c r="B244">
+        <v>65</v>
+      </c>
+      <c r="E244">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>3</v>
+      </c>
+      <c r="B245">
+        <v>66</v>
+      </c>
+      <c r="C245">
+        <v>45</v>
+      </c>
+      <c r="D245">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="E245">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>3</v>
+      </c>
+      <c r="B246">
+        <v>67</v>
+      </c>
+      <c r="E246">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>3</v>
+      </c>
+      <c r="B247">
+        <v>68</v>
+      </c>
+      <c r="E247">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>3</v>
+      </c>
+      <c r="B248">
+        <v>69</v>
+      </c>
+      <c r="C248">
+        <v>40</v>
+      </c>
+      <c r="D248">
+        <f t="shared" si="5"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="E248">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>3</v>
+      </c>
+      <c r="B249">
+        <v>70</v>
+      </c>
+      <c r="C249">
+        <v>27</v>
+      </c>
+      <c r="D249">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="E249">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>3</v>
+      </c>
+      <c r="B250">
+        <v>71</v>
+      </c>
+      <c r="C250">
+        <v>47</v>
+      </c>
+      <c r="D250">
+        <f t="shared" si="5"/>
+        <v>15.666666666666666</v>
+      </c>
+      <c r="E250">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>3</v>
+      </c>
+      <c r="B251">
+        <v>72</v>
+      </c>
+      <c r="E251">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>3</v>
+      </c>
+      <c r="B252">
+        <v>73</v>
+      </c>
+      <c r="E252">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>3</v>
+      </c>
+      <c r="B253">
+        <v>74</v>
+      </c>
+      <c r="E253">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>3</v>
+      </c>
+      <c r="B254">
+        <v>75</v>
+      </c>
+      <c r="E254">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>3</v>
+      </c>
+      <c r="B255">
+        <v>76</v>
+      </c>
+      <c r="C255">
+        <v>33</v>
+      </c>
+      <c r="D255">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="E255">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>3</v>
+      </c>
+      <c r="B256">
+        <v>77</v>
+      </c>
+      <c r="C256">
+        <v>42</v>
+      </c>
+      <c r="D256">
+        <f>SUM(C256)/3</f>
+        <v>14</v>
+      </c>
+      <c r="E256">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>3</v>
+      </c>
+      <c r="B257">
+        <v>78</v>
+      </c>
+      <c r="C257">
+        <v>38</v>
+      </c>
+      <c r="D257">
+        <f t="shared" si="5"/>
+        <v>12.666666666666666</v>
+      </c>
+      <c r="E257">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>3</v>
+      </c>
+      <c r="B258">
+        <v>79</v>
+      </c>
+      <c r="E258">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>3</v>
+      </c>
+      <c r="B259">
+        <v>80</v>
+      </c>
+      <c r="C259">
+        <v>22</v>
+      </c>
+      <c r="D259">
+        <f t="shared" si="5"/>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="E259">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>3</v>
+      </c>
+      <c r="B260">
+        <v>81</v>
+      </c>
+      <c r="E260">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>3</v>
+      </c>
+      <c r="B261">
+        <v>82</v>
+      </c>
+      <c r="C261">
+        <v>39</v>
+      </c>
+      <c r="D261">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="E261">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>3</v>
+      </c>
+      <c r="B262">
+        <v>83</v>
+      </c>
+      <c r="C262">
+        <v>43</v>
+      </c>
+      <c r="D262">
+        <f t="shared" si="5"/>
+        <v>14.333333333333334</v>
+      </c>
+      <c r="E262">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>3</v>
+      </c>
+      <c r="B263">
+        <v>84</v>
+      </c>
+      <c r="E263">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>3</v>
+      </c>
+      <c r="B264">
+        <v>85</v>
+      </c>
+      <c r="C264">
+        <v>46</v>
+      </c>
+      <c r="D264">
+        <f t="shared" si="5"/>
+        <v>15.333333333333334</v>
+      </c>
+      <c r="E264">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>3</v>
+      </c>
+      <c r="B265">
+        <v>86</v>
+      </c>
+      <c r="E265">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>3</v>
+      </c>
+      <c r="B266">
+        <v>87</v>
+      </c>
+      <c r="C266">
+        <v>49</v>
+      </c>
+      <c r="D266">
+        <f>SUM(C266)/4</f>
+        <v>12.25</v>
+      </c>
+      <c r="E266">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>1</v>
+      </c>
+      <c r="B267">
+        <v>18</v>
+      </c>
+      <c r="E267">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>1</v>
+      </c>
+      <c r="B268">
+        <v>19</v>
+      </c>
+      <c r="C268">
+        <v>42</v>
+      </c>
+      <c r="D268">
+        <f>SUM(C268)/3</f>
+        <v>14</v>
+      </c>
+      <c r="E268">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>1</v>
+      </c>
+      <c r="B269">
+        <v>20</v>
+      </c>
+      <c r="E269">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>1</v>
+      </c>
+      <c r="B270">
+        <v>21</v>
+      </c>
+      <c r="E270">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>1</v>
+      </c>
+      <c r="B271">
+        <v>22</v>
+      </c>
+      <c r="C271">
+        <v>32</v>
+      </c>
+      <c r="D271">
+        <f t="shared" ref="D269:D319" si="6">SUM(C271)/3</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="E271">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>1</v>
+      </c>
+      <c r="B272">
+        <v>23</v>
+      </c>
+      <c r="E272">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>1</v>
+      </c>
+      <c r="B273">
+        <v>24</v>
+      </c>
+      <c r="E273">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>1</v>
+      </c>
+      <c r="B274">
+        <v>25</v>
+      </c>
+      <c r="E274">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>1</v>
+      </c>
+      <c r="B275">
+        <v>26</v>
+      </c>
+      <c r="C275">
+        <v>0</v>
+      </c>
+      <c r="D275">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E275">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>1</v>
+      </c>
+      <c r="B276">
+        <v>27</v>
+      </c>
+      <c r="C276">
+        <v>32</v>
+      </c>
+      <c r="D276">
+        <f t="shared" si="6"/>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="E276">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>1</v>
+      </c>
+      <c r="B277">
+        <v>28</v>
+      </c>
+      <c r="E277">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>1</v>
+      </c>
+      <c r="B278">
+        <v>29</v>
+      </c>
+      <c r="E278">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>1</v>
+      </c>
+      <c r="B279">
+        <v>30</v>
+      </c>
+      <c r="C279">
+        <v>37</v>
+      </c>
+      <c r="D279">
+        <f t="shared" si="6"/>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="E279">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>1</v>
+      </c>
+      <c r="B280">
+        <v>31</v>
+      </c>
+      <c r="C280">
+        <v>30</v>
+      </c>
+      <c r="D280">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="E280">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>1</v>
+      </c>
+      <c r="B281">
+        <v>32</v>
+      </c>
+      <c r="C281">
+        <v>35</v>
+      </c>
+      <c r="D281">
+        <f t="shared" si="6"/>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="E281">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>1</v>
+      </c>
+      <c r="B282">
+        <v>33</v>
+      </c>
+      <c r="E282">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>1</v>
+      </c>
+      <c r="B283">
+        <v>34</v>
+      </c>
+      <c r="E283">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A284" t="s">
+        <v>1</v>
+      </c>
+      <c r="B284">
+        <v>35</v>
+      </c>
+      <c r="C284">
+        <v>0</v>
+      </c>
+      <c r="D284">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E284">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
+        <v>1</v>
+      </c>
+      <c r="B285">
+        <v>36</v>
+      </c>
+      <c r="E285">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>1</v>
+      </c>
+      <c r="B286">
+        <v>37</v>
+      </c>
+      <c r="C286">
+        <v>46</v>
+      </c>
+      <c r="D286">
+        <f t="shared" si="6"/>
+        <v>15.333333333333334</v>
+      </c>
+      <c r="E286">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A287" t="s">
+        <v>1</v>
+      </c>
+      <c r="B287">
+        <v>38</v>
+      </c>
+      <c r="E287">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A288" t="s">
+        <v>1</v>
+      </c>
+      <c r="B288">
+        <v>39</v>
+      </c>
+      <c r="E288">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
+        <v>1</v>
+      </c>
+      <c r="B289">
+        <v>40</v>
+      </c>
+      <c r="C289">
+        <v>0</v>
+      </c>
+      <c r="D289">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E289">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
+        <v>1</v>
+      </c>
+      <c r="B290">
+        <v>41</v>
+      </c>
+      <c r="E290">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A291" t="s">
+        <v>1</v>
+      </c>
+      <c r="B291">
+        <v>42</v>
+      </c>
+      <c r="E291">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A292" t="s">
+        <v>1</v>
+      </c>
+      <c r="B292">
+        <v>43</v>
+      </c>
+      <c r="E292">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A293" t="s">
+        <v>1</v>
+      </c>
+      <c r="B293">
+        <v>44</v>
+      </c>
+      <c r="C293">
+        <v>8</v>
+      </c>
+      <c r="D293">
+        <f t="shared" si="6"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="E293">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A294" t="s">
+        <v>3</v>
+      </c>
+      <c r="B294">
+        <v>62</v>
+      </c>
+      <c r="E294">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A295" t="s">
+        <v>3</v>
+      </c>
+      <c r="B295">
+        <v>63</v>
+      </c>
+      <c r="C295">
+        <v>0</v>
+      </c>
+      <c r="D295">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E295">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A296" t="s">
+        <v>3</v>
+      </c>
+      <c r="B296">
+        <v>64</v>
+      </c>
+      <c r="E296">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A297" t="s">
+        <v>3</v>
+      </c>
+      <c r="B297">
+        <v>65</v>
+      </c>
+      <c r="E297">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A298" t="s">
+        <v>3</v>
+      </c>
+      <c r="B298">
+        <v>66</v>
+      </c>
+      <c r="C298">
+        <v>30</v>
+      </c>
+      <c r="D298">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="E298">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A299" t="s">
+        <v>3</v>
+      </c>
+      <c r="B299">
+        <v>67</v>
+      </c>
+      <c r="E299">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A300" t="s">
+        <v>3</v>
+      </c>
+      <c r="B300">
+        <v>68</v>
+      </c>
+      <c r="E300">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A301" t="s">
+        <v>3</v>
+      </c>
+      <c r="B301">
+        <v>69</v>
+      </c>
+      <c r="E301">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A302" t="s">
+        <v>3</v>
+      </c>
+      <c r="B302">
+        <v>70</v>
+      </c>
+      <c r="C302">
+        <v>0</v>
+      </c>
+      <c r="D302">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E302">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A303" t="s">
+        <v>3</v>
+      </c>
+      <c r="B303">
+        <v>71</v>
+      </c>
+      <c r="C303">
+        <v>0</v>
+      </c>
+      <c r="D303">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E303">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A304" t="s">
+        <v>3</v>
+      </c>
+      <c r="B304">
+        <v>72</v>
+      </c>
+      <c r="E304">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A305" t="s">
+        <v>3</v>
+      </c>
+      <c r="B305">
+        <v>73</v>
+      </c>
+      <c r="E305">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A306" t="s">
+        <v>3</v>
+      </c>
+      <c r="B306">
+        <v>74</v>
+      </c>
+      <c r="E306">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A307" t="s">
+        <v>3</v>
+      </c>
+      <c r="B307">
+        <v>75</v>
+      </c>
+      <c r="E307">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A308" t="s">
+        <v>3</v>
+      </c>
+      <c r="B308">
+        <v>76</v>
+      </c>
+      <c r="C308">
+        <v>18</v>
+      </c>
+      <c r="D308">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="E308">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A309" t="s">
+        <v>3</v>
+      </c>
+      <c r="B309">
+        <v>77</v>
+      </c>
+      <c r="C309">
+        <v>49</v>
+      </c>
+      <c r="D309">
+        <f t="shared" si="6"/>
+        <v>16.333333333333332</v>
+      </c>
+      <c r="E309">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A310" t="s">
+        <v>3</v>
+      </c>
+      <c r="B310">
+        <v>78</v>
+      </c>
+      <c r="C310">
+        <v>0</v>
+      </c>
+      <c r="D310">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E310">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A311" t="s">
+        <v>3</v>
+      </c>
+      <c r="B311">
+        <v>79</v>
+      </c>
+      <c r="E311">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A312" t="s">
+        <v>3</v>
+      </c>
+      <c r="B312">
+        <v>80</v>
+      </c>
+      <c r="C312">
+        <v>2</v>
+      </c>
+      <c r="D312">
+        <f t="shared" si="6"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E312">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A313" t="s">
+        <v>3</v>
+      </c>
+      <c r="B313">
+        <v>81</v>
+      </c>
+      <c r="E313">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A314" t="s">
+        <v>3</v>
+      </c>
+      <c r="B314">
+        <v>82</v>
+      </c>
+      <c r="C314">
+        <v>0</v>
+      </c>
+      <c r="D314">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E314">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A315" t="s">
+        <v>3</v>
+      </c>
+      <c r="B315">
+        <v>83</v>
+      </c>
+      <c r="E315">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A316" t="s">
+        <v>3</v>
+      </c>
+      <c r="B316">
+        <v>84</v>
+      </c>
+      <c r="E316">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A317" t="s">
+        <v>3</v>
+      </c>
+      <c r="B317">
+        <v>85</v>
+      </c>
+      <c r="E317">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A318" t="s">
+        <v>3</v>
+      </c>
+      <c r="B318">
+        <v>86</v>
+      </c>
+      <c r="E318">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A319" t="s">
+        <v>3</v>
+      </c>
+      <c r="B319">
+        <v>87</v>
+      </c>
+      <c r="C319">
+        <v>56</v>
+      </c>
+      <c r="D319">
+        <f t="shared" si="6"/>
+        <v>18.666666666666668</v>
+      </c>
+      <c r="E319">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>